<commit_message>
Final Review and Editing
Rewrote some things in the log hours sheet and uploaded the build as well (just in case).
</commit_message>
<xml_diff>
--- a/LogHours.xlsx
+++ b/LogHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drilo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drilo\Desktop\Maze-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFCDA37-454D-44CE-A7EE-05019F9C83DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835F80EC-BFAC-4EAB-A756-1374F5E51C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Subject</t>
   </si>
@@ -76,52 +76,121 @@
     <t>Bonus</t>
   </si>
   <si>
-    <t>Research &amp; Approach</t>
-  </si>
-  <si>
     <t>Coding Camera Pan Script</t>
   </si>
   <si>
     <t>Coding Maze Generator</t>
   </si>
   <si>
-    <t xml:space="preserve">After deciding on how to render the walls and cells of the maze, I thought of creating a camera pan script, in order to move it around the maze and within the maze's bounds. This is not related to the maze generation algorithm at all, however it is done for moving around the maze and it fixes the FPS problems of rendering all cells at once to the camera. </t>
-  </si>
-  <si>
-    <t>After choosing the option for maze generation with selecting frontier neighbours and skiping the adjacient ones, I started coding the algorithm and created the Cell prefab and some materials that I needed for coloring walls and passages.</t>
-  </si>
-  <si>
-    <t>Debugging Maze Generator Code</t>
-  </si>
-  <si>
-    <t>Googled about Prim's algorithm, and checked some maze generation examples on YouTube. This one *video got my attention and decided to do it this way, a maze with thick wall.  (Link to video : https://www.youtube.com/watch?v=Vo-oXdS6atk&amp;t=229s) Regarding the size requirements of the maze, I wanted to find a good approach at the beginning, for showin only some part of the maze because showing it all at once when on large dimensions would not look good and would probably lower the FPS due to the way I wanted to create it. I will write the code from scratch based on this pseduo code of how the Prim's algorithm works. (Link to pseudo code https://stackoverflow.com/questions/29739751/implementing-a-randomly-generated-maze-using-prims-algorithm) first response to the questions*.</t>
-  </si>
-  <si>
-    <t>After coding the generation of grid cells and the maze generator algorithm, I had to debug some erros with indexes and managed to fix it. However, because of how I am doing the maze generation now (skipping the adjacent nighbour and getting the frontier neighbour), when giving even number of dimensions, there would always be an unprocessed line of cells (double walls on the max width and height). To fix this issues, I added an extra cell row if the given dimension number of that axe was even.</t>
-  </si>
-  <si>
-    <t>Creating the other type of maze with thin walls</t>
-  </si>
-  <si>
-    <t>After realising the issues of given even dimension numbers, I decided to create a maze with thin walls which would eradicate the issue of giving even dimension numbers. I had to edit the Cell prefab and add 4 line renders (one per wall, North, South, East and West). I use the same Cell prefab for both modes (slim and thick walls), but based on the given condition, I enable and disable the main background sprite renderer and line renderers (walls).</t>
-  </si>
-  <si>
     <t>Creating the UI</t>
   </si>
   <si>
-    <t>Created the UI and made it scalable between the 3 given resolutions of Desktop, iPhone and iPad</t>
-  </si>
-  <si>
     <t>Refactored and Cleaned Code</t>
   </si>
   <si>
-    <t>After making it work for both modes without any errors, I decided to make the code reusable, wrote down comments to explain some parts that might be confusing to others and deleted some uneccessary lines of code that I previously thought were necessary.</t>
-  </si>
-  <si>
     <t>Animating the maze generation</t>
   </si>
   <si>
-    <t>Turned the maze generation algorithm into a coroutine so to animate the ways of how the algorithm works</t>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>I did some research on the algorithms used to generate mazes, apparently there are many algorithms that can be used. Most of them are are normal in terms of relative speed, the fastest being Binary Tree Maze and it having a diagonal basis, which makes it have a repetitive patterns of binary partition of paths. The Prim's algorithm, although considered to be hard to implement, it is fast and generates a consistent randomness of maze paths, not too many straight paths, but having more turns and dead ends and making it harder to solve. 
+I searched on YouTube about how other programmers have implemented and visualized the algorithm, and later on found the pseudo algorithm code and decided to write everything from scratch by using the pseudo code as a template. 
+Link -  https://people.cs.ksu.edu/~ashley78/wiki.ashleycoleman.me/index.php/Prim's_Algorithm.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The first issue that I ran into when thinking of an approach to this problem, was the maximum size of the maze dimensions (250x250). There were two solutions I could think of. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Solution 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Create individual cells, each one is a game object with a SpriteRenderer component, and color it based on whether it is a wall or passge. The downside of this is, if shown all in one screen, then the FPS would drop down to around 15. The counter-argument to this issue is that showing the entire maze on the screen would make it small and hard to see because of the camera being at a greater distance, so by having the same camera zoom at all time, we do not need to render all of the cells at once.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>Solution 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Render the maze on a texture based on the data from the grid of cells. This seemed as a promising solution, yet the issue of camera being far away in order to show the whole maze somehow made me think of it twice before going on, since it is the same issue that the first solution has. Nonetheless, having controll and keeping data within a single cell on its own, makes it easier to develop further functionalities if I want to.
+I did a research on both solutions, for any other extra information that I might have not thought about and at the end decided I will go with the first solution. </t>
+    </r>
+  </si>
+  <si>
+    <t>While researching about other's maze generation algorithm implementation and visualization, I got interested more on the type of maze with walls having the same thickenss as passages (isometric).
+To do this type of maze, I had to skip the adjacent neighbours of a cell and get the frontier neighbours (skipping a neighbour), because the adjacent neighbours can be of wall or passage type cellsm meanwhile the frontier neighbours can only be of passage type cells.
+The downside of this is that dimensions of even numbers will not work good, since if given dimensions are even numbers, there will always be a wasted line of frontier neighbour cells, along the horizontal and vertical axes. However, I decided to go on with this since I could easily implement a thin wall type of maze with less effort based on the code for thick wall maze generation.
+Link to youtube video that gave me the idea of generating an isometric maze 
+https://www.youtube.com/watch?v=Vo-oXdS6atk&amp;t=229s</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After coding most of the needed functionalities and doing a lot of indexing maths (simple, yet easily to mistake kind of maths), the switching of cell colors based on the type, finding neighbours of cells and joining cells, etc, it was more than expected for it to not work the first try, so I had to debug some errors with index addition and subtraction, after some time I managed to fix it.
+Moreover, after debugging the code, the dimensions of even numbers started to get into my mind as I was thinking of a solution to fix it, so right after finishing the thick wall type maze generator, I decided to generate a maze with thin/slim walls.
+</t>
+  </si>
+  <si>
+    <t>Thin/Slim Walls Maze Generator (Coding)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After deciding that I want to go with the first soultion, I need to code a camera panner so we can move around the maze if its dimensions are bigger than the surface the camera can show at once, without losing quality and details.
+I found a good basis script about camera panning, however, I had to code the constraining of camera position. I wanted to pan the camera around and not go off maze bounds at the same time.
+I had to take into account the screen resoultion as well, because it was asked that the UI should scale up correctly when using the Desktop, iPhone and iPad resolutions.
+So instead of making it work only for these screen resolutions, I decided to automate it and make it functional for every kind of screen resolution.
+Link to the base camera pan script: 
+https://www.codegrepper.com/code-examples/csharp/scroll+and+pan+2d+camera+unity
+</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After realising the issues of given even dimension numbers, I decided to create a maze with thin walls which would eradicate the issue of giving even dimension numbers. 
+I added 4 line renders to the Cell prefab (one per wall, North, South, East and West). I use the same Cell prefab for both modes (slim and thick walls), but based on the given condition, I enable and disable the main background sprite renderer and line renderers (walls). 
+At first I was worried about the FPS dropping more due to have 4 lines being rendered instead of just one sprite, however, when the maze is generated, not all the walls will be active so the number of FPS will not have a huge downdrop by goind under 60.
+</t>
+  </si>
+  <si>
+    <t>Created the UI and made it scalable between the 3 given resolutions of Desktop, iPhone and iPad. I added the animation speed slide (0 to 1 second) since it would not make sense to wait more than 1 seconds per step, since it is easily understandable with 1 second setps.</t>
+  </si>
+  <si>
+    <t>After making it work for both modes without any errors, I decided to make the code reusable, wrote down comments to explain some parts that might be confusing to others and deleted some uneccessary lines of code that I previously thought were necessary. The optimisations were done within reason and I tried to not start changing all the code completely since that would introduce way more bugs.</t>
+  </si>
+  <si>
+    <t>Turned the maze generation algorithm into a coroutine so to animate the ways of how the algorithm works, step by step.</t>
   </si>
 </sst>
 </file>
@@ -210,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEB5340"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +499,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -448,9 +523,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -458,18 +530,9 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +544,34 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1739,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1756,345 +1847,373 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="156" x14ac:dyDescent="0.4">
+      <c r="A5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="28">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29">
+        <v>44531</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="216" x14ac:dyDescent="0.4">
+      <c r="A6" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="28">
+        <v>1</v>
+      </c>
+      <c r="C6" s="29">
+        <v>44531</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="192" x14ac:dyDescent="0.4">
+      <c r="A7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B7" s="28">
         <v>2</v>
       </c>
-      <c r="C4" s="18">
-        <v>44531</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
+      <c r="C7" s="29">
+        <v>44532</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="180" x14ac:dyDescent="0.4">
+      <c r="A8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B8" s="28">
+        <v>3</v>
+      </c>
+      <c r="C8" s="29">
+        <v>44532</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.4">
+      <c r="A9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
-        <v>44532</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C9" s="29">
+        <v>44533</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="144" x14ac:dyDescent="0.4">
+      <c r="A10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="28">
+        <v>3</v>
+      </c>
+      <c r="C10" s="29">
+        <v>44535</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.4">
+      <c r="A11" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="28">
+        <v>1</v>
+      </c>
+      <c r="C11" s="29">
+        <v>44535</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.4">
+      <c r="A12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="17">
-        <v>3</v>
-      </c>
-      <c r="C6" s="18">
-        <v>44532</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="B12" s="28">
+        <v>2</v>
+      </c>
+      <c r="C12" s="29">
+        <v>44536</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.4">
+      <c r="A13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="97.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="17">
-        <v>2</v>
-      </c>
-      <c r="C7" s="18">
-        <v>44533</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="17">
-        <v>2</v>
-      </c>
-      <c r="C8" s="18">
-        <v>44535</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="17">
-        <v>2</v>
-      </c>
-      <c r="C9" s="18">
-        <v>44535</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="17">
-        <v>2</v>
-      </c>
-      <c r="C10" s="18">
+      <c r="B13" s="16"/>
+      <c r="C13" s="17">
         <v>44536</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
+      <c r="D13" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="20"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="20"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="20"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="20"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A26" s="5"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="20"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A27" s="5"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A28" s="5"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="20"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="3"/>
+    <row r="29" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A29" s="5"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="14">
-        <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>15</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+    <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A30" s="5"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+    <row r="31" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="3"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="3"/>
+    <row r="32" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="14">
+        <f>SUMIF(E5:E30,"&lt;&gt;x",B5:B30)</f>
+        <v>15</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>